<commit_message>
changed figures and tested analyses for ms revisions
</commit_message>
<xml_diff>
--- a/data/2021-06-26_AgNPs-fish-excretion-models-simulation.xlsx
+++ b/data/2021-06-26_AgNPs-fish-excretion-models-simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklem\Documents\Etudes\Trent\Xenopoulos lab\Projects\AgNP ELA lakes &amp; fish excretion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/AgNP-ELA_fish-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{9BCFF35B-EB1F-4DD7-8071-5B75C796A948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="21 05 12 AgNP fish excretion mo" sheetId="1" r:id="rId1"/>
@@ -2412,7 +2412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>

</xml_diff>